<commit_message>
correct the name of Demo chair and remove duplicates from PC members
</commit_message>
<xml_diff>
--- a/PC members.xlsx
+++ b/PC members.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowWidth="21240" windowHeight="11860"/>
+    <workbookView windowWidth="28800" windowHeight="11860"/>
   </bookViews>
   <sheets>
     <sheet name="sort by last name" sheetId="1" r:id="rId1"/>
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="140">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="143">
   <si>
     <t>first name</t>
   </si>
@@ -92,6 +92,15 @@
   </si>
   <si>
     <t>Chavan</t>
+  </si>
+  <si>
+    <t>Soura</t>
+  </si>
+  <si>
+    <t>Dasgupta</t>
+  </si>
+  <si>
+    <t>University of Iowa</t>
   </si>
   <si>
     <t>Shawfeng</t>
@@ -441,12 +450,12 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="4">
+    <numFmt numFmtId="41" formatCode="_-* #,##0_-;\-* #,##0_-;_-* &quot;-&quot;_-;_-@_-"/>
+    <numFmt numFmtId="42" formatCode="_-&quot;£&quot;* #,##0_-;\-&quot;£&quot;* #,##0_-;_-&quot;£&quot;* &quot;-&quot;_-;_-@_-"/>
+    <numFmt numFmtId="44" formatCode="_-&quot;£&quot;* #,##0.00_-;\-&quot;£&quot;* #,##0.00_-;_-&quot;£&quot;* &quot;-&quot;??_-;_-@_-"/>
     <numFmt numFmtId="43" formatCode="_-* #,##0.00_-;\-* #,##0.00_-;_-* &quot;-&quot;??_-;_-@_-"/>
-    <numFmt numFmtId="44" formatCode="_-&quot;£&quot;* #,##0.00_-;\-&quot;£&quot;* #,##0.00_-;_-&quot;£&quot;* &quot;-&quot;??_-;_-@_-"/>
-    <numFmt numFmtId="42" formatCode="_-&quot;£&quot;* #,##0_-;\-&quot;£&quot;* #,##0_-;_-&quot;£&quot;* &quot;-&quot;_-;_-@_-"/>
-    <numFmt numFmtId="41" formatCode="_-* #,##0_-;\-* #,##0_-;_-* &quot;-&quot;_-;_-@_-"/>
   </numFmts>
-  <fonts count="22">
+  <fonts count="23">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -467,8 +476,45 @@
       <charset val="134"/>
     </font>
     <font>
+      <sz val="9"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <sz val="11"/>
       <color theme="0"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF800080"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -483,42 +529,10 @@
     </font>
     <font>
       <b/>
-      <sz val="18"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
       <sz val="11"/>
-      <color rgb="FF800080"/>
+      <color rgb="FFFA7D00"/>
       <name val="Calibri"/>
       <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <i/>
-      <sz val="11"/>
-      <color rgb="FF7F7F7F"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="13"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -529,23 +543,9 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <u/>
+      <b/>
       <sz val="11"/>
-      <color rgb="FF0000FF"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C6500"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="1"/>
+      <color rgb="FF3F3F3F"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -566,6 +566,13 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <sz val="11"/>
+      <color rgb="FF9C0006"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <b/>
       <sz val="15"/>
       <color theme="3"/>
@@ -575,15 +582,7 @@
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FFFF0000"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FF3F3F3F"/>
+      <color rgb="FF9C6500"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -596,16 +595,33 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <b/>
+      <sz val="18"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
       <sz val="11"/>
-      <color rgb="FF9C0006"/>
+      <color rgb="FF0000FF"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
       <b/>
+      <sz val="13"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <i/>
       <sz val="11"/>
-      <color rgb="FFFA7D00"/>
+      <color rgb="FF7F7F7F"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -626,187 +642,187 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="6" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
+        <fgColor theme="7" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="9"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -817,6 +833,15 @@
       <right/>
       <top/>
       <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4" tint="0.499984740745262"/>
+      </bottom>
       <diagonal/>
     </border>
     <border>
@@ -831,24 +856,6 @@
       </top>
       <bottom style="double">
         <color rgb="FF3F3F3F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4" tint="0.499984740745262"/>
       </bottom>
       <diagonal/>
     </border>
@@ -883,17 +890,6 @@
       <diagonal/>
     </border>
     <border>
-      <left/>
-      <right/>
-      <top style="thin">
-        <color theme="4"/>
-      </top>
-      <bottom style="double">
-        <color theme="4"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
       <left style="thin">
         <color rgb="FF3F3F3F"/>
       </left>
@@ -911,6 +907,26 @@
     <border>
       <left/>
       <right/>
+      <top style="thin">
+        <color theme="4"/>
+      </top>
+      <bottom style="double">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
       <top/>
       <bottom style="double">
         <color rgb="FFFF8001"/>
@@ -922,152 +938,152 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="26" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="6" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="8" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="44" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="5" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="7" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="26" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="4" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="11" borderId="4" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="9" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="10" fillId="8" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="41" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="4" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="42" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="42" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="43" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="5" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="9" fillId="6" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -1085,6 +1101,9 @@
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1">
+      <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
@@ -1408,12 +1427,12 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
   <sheetPr/>
-  <dimension ref="A1:E50"/>
+  <dimension ref="A1:E51"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="170" zoomScaleNormal="170" topLeftCell="C1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+    <sheetView tabSelected="1" zoomScale="170" zoomScaleNormal="170" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A12" activePane="bottomLeft" state="frozen"/>
       <selection/>
-      <selection pane="bottomLeft" activeCell="E50" sqref="E2:E50"/>
+      <selection pane="bottomLeft" activeCell="E12" sqref="E12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.14285714285714" defaultRowHeight="11.6" outlineLevelCol="4"/>
@@ -1449,7 +1468,7 @@
         <v>5</v>
       </c>
       <c r="E2" s="1" t="str">
-        <f>CONCATENATE("**",A2," ",B2,"** ",C2,D2)</f>
+        <f t="shared" ref="E2:E52" si="0">CONCATENATE("**",A2," ",B2,"** ",C2,D2)</f>
         <v>**Peter Baumann** Jacobs University Bremen&lt;br&gt;</v>
       </c>
     </row>
@@ -1467,7 +1486,7 @@
         <v>5</v>
       </c>
       <c r="E3" s="1" t="str">
-        <f t="shared" ref="E3:E50" si="0">CONCATENATE("**",A3," ",B3,"** ",C3,D3)</f>
+        <f t="shared" si="0"/>
         <v>**Khalid Belhajjame** PSL, Université Paris-Dauphine, LAMSADE, France&lt;br&gt;</v>
       </c>
     </row>
@@ -1580,31 +1599,31 @@
       </c>
     </row>
     <row r="10" ht="12" spans="1:5">
-      <c r="A10" s="1" t="s">
+      <c r="A10" s="6" t="s">
         <v>26</v>
       </c>
-      <c r="B10" s="1" t="s">
+      <c r="B10" s="6" t="s">
         <v>27</v>
       </c>
-      <c r="C10" s="5" t="s">
-        <v>14</v>
+      <c r="C10" s="6" t="s">
+        <v>28</v>
       </c>
       <c r="D10" s="1" t="s">
         <v>5</v>
       </c>
       <c r="E10" s="1" t="str">
         <f t="shared" si="0"/>
-        <v>**Shawfeng Dong** Lawrence Berkeley National Laboratory&lt;br&gt;</v>
+        <v>**Soura Dasgupta** University of Iowa&lt;br&gt;</v>
       </c>
     </row>
     <row r="11" ht="12" spans="1:5">
       <c r="A11" s="1" t="s">
-        <v>28</v>
-      </c>
-      <c r="B11" s="4" t="s">
-        <v>27</v>
-      </c>
-      <c r="C11" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="B11" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="C11" s="5" t="s">
         <v>14</v>
       </c>
       <c r="D11" s="1" t="s">
@@ -1612,25 +1631,25 @@
       </c>
       <c r="E11" s="1" t="str">
         <f t="shared" si="0"/>
-        <v>**Bin Dong** Lawrence Berkeley National Laboratory&lt;br&gt;</v>
+        <v>**Shawfeng Dong** Lawrence Berkeley National Laboratory&lt;br&gt;</v>
       </c>
     </row>
     <row r="12" ht="12" spans="1:5">
       <c r="A12" s="1" t="s">
-        <v>29</v>
-      </c>
-      <c r="B12" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="B12" s="4" t="s">
         <v>30</v>
       </c>
-      <c r="C12" s="5" t="s">
-        <v>31</v>
+      <c r="C12" s="1" t="s">
+        <v>14</v>
       </c>
       <c r="D12" s="1" t="s">
         <v>5</v>
       </c>
       <c r="E12" s="1" t="str">
         <f t="shared" si="0"/>
-        <v>**Ahmed Eldawy** University of California, Riverside&lt;br&gt;</v>
+        <v>**Bin Dong** Lawrence Berkeley National Laboratory&lt;br&gt;</v>
       </c>
     </row>
     <row r="13" ht="12" spans="1:5">
@@ -1648,7 +1667,7 @@
       </c>
       <c r="E13" s="1" t="str">
         <f t="shared" si="0"/>
-        <v>**Jan Foster** University of Chicago&lt;br&gt;</v>
+        <v>**Ahmed Eldawy** University of California, Riverside&lt;br&gt;</v>
       </c>
     </row>
     <row r="14" ht="12" spans="1:5">
@@ -1666,7 +1685,7 @@
       </c>
       <c r="E14" s="1" t="str">
         <f t="shared" si="0"/>
-        <v>**Marios Fragkoulis** Delft University of Technology, The Netherlands&lt;br&gt;</v>
+        <v>**Jan Foster** University of Chicago&lt;br&gt;</v>
       </c>
     </row>
     <row r="15" ht="12" spans="1:5">
@@ -1684,7 +1703,7 @@
       </c>
       <c r="E15" s="1" t="str">
         <f t="shared" si="0"/>
-        <v>**Filippo Furfaro** DIMES - University of Calabria, Italy&lt;br&gt;</v>
+        <v>**Marios Fragkoulis** Delft University of Technology, The Netherlands&lt;br&gt;</v>
       </c>
     </row>
     <row r="16" ht="12" spans="1:5">
@@ -1702,43 +1721,43 @@
       </c>
       <c r="E16" s="1" t="str">
         <f t="shared" si="0"/>
+        <v>**Filippo Furfaro** DIMES - University of Calabria, Italy&lt;br&gt;</v>
+      </c>
+    </row>
+    <row r="17" ht="12" spans="1:5">
+      <c r="A17" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="B17" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="C17" s="5" t="s">
+        <v>46</v>
+      </c>
+      <c r="D17" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="E17" s="1" t="str">
+        <f t="shared" si="0"/>
         <v>**Lukasz Golab** University of Waterloo&lt;br&gt;</v>
       </c>
     </row>
-    <row r="17" ht="12" spans="1:5">
-      <c r="A17" s="6" t="s">
-        <v>44</v>
-      </c>
-      <c r="B17" s="6" t="s">
-        <v>45</v>
-      </c>
-      <c r="C17" s="6" t="s">
-        <v>46</v>
-      </c>
-      <c r="D17" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="E17" s="1" t="str">
+    <row r="18" ht="12" spans="1:5">
+      <c r="A18" s="7" t="s">
+        <v>47</v>
+      </c>
+      <c r="B18" s="7" t="s">
+        <v>48</v>
+      </c>
+      <c r="C18" s="7" t="s">
+        <v>49</v>
+      </c>
+      <c r="D18" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="E18" s="1" t="str">
         <f t="shared" si="0"/>
         <v>**Peiquan Jin** University of Science and Technology of China&lt;br&gt;</v>
-      </c>
-    </row>
-    <row r="18" ht="12" spans="1:5">
-      <c r="A18" s="1" t="s">
-        <v>47</v>
-      </c>
-      <c r="B18" s="1" t="s">
-        <v>48</v>
-      </c>
-      <c r="C18" s="5" t="s">
-        <v>49</v>
-      </c>
-      <c r="D18" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="E18" s="1" t="str">
-        <f t="shared" si="0"/>
-        <v>**Verena Kantere** University of Ottawa&lt;br&gt;</v>
       </c>
     </row>
     <row r="19" ht="12" spans="1:5">
@@ -1756,7 +1775,7 @@
       </c>
       <c r="E19" s="1" t="str">
         <f t="shared" si="0"/>
-        <v>**Zoi Kaoudi** Technische Universität Berlin, Germany&lt;br&gt;</v>
+        <v>**Verena Kantere** University of Ottawa&lt;br&gt;</v>
       </c>
     </row>
     <row r="20" ht="12" spans="1:5">
@@ -1774,7 +1793,7 @@
       </c>
       <c r="E20" s="1" t="str">
         <f t="shared" si="0"/>
-        <v>**Jinoh Kim** Texas A&amp;M University-Commerce&lt;br&gt;</v>
+        <v>**Zoi Kaoudi** Technische Universität Berlin, Germany&lt;br&gt;</v>
       </c>
     </row>
     <row r="21" ht="12" spans="1:5">
@@ -1792,7 +1811,7 @@
       </c>
       <c r="E21" s="1" t="str">
         <f t="shared" si="0"/>
-        <v>**Seokki Lee** University of Cincinnati&lt;br&gt;</v>
+        <v>**Jinoh Kim** Texas A&amp;M University-Commerce&lt;br&gt;</v>
       </c>
     </row>
     <row r="22" ht="12" spans="1:5">
@@ -1810,17 +1829,17 @@
       </c>
       <c r="E22" s="1" t="str">
         <f t="shared" si="0"/>
-        <v>**Ulf Leser** Humboldt-Universität zu Berlin, Germany&lt;br&gt;</v>
+        <v>**Seokki Lee** University of Cincinnati&lt;br&gt;</v>
       </c>
     </row>
     <row r="23" ht="12" spans="1:5">
       <c r="A23" s="1" t="s">
         <v>62</v>
       </c>
-      <c r="B23" s="4" t="s">
+      <c r="B23" s="1" t="s">
         <v>63</v>
       </c>
-      <c r="C23" s="1" t="s">
+      <c r="C23" s="5" t="s">
         <v>64</v>
       </c>
       <c r="D23" s="1" t="s">
@@ -1828,17 +1847,17 @@
       </c>
       <c r="E23" s="1" t="str">
         <f t="shared" si="0"/>
-        <v>**Xin Liang** Oak Ridge National Laboratory&lt;br&gt;</v>
+        <v>**Ulf Leser** Humboldt-Universität zu Berlin, Germany&lt;br&gt;</v>
       </c>
     </row>
     <row r="24" ht="12" spans="1:5">
       <c r="A24" s="1" t="s">
         <v>65</v>
       </c>
-      <c r="B24" s="1" t="s">
+      <c r="B24" s="4" t="s">
         <v>66</v>
       </c>
-      <c r="C24" s="5" t="s">
+      <c r="C24" s="1" t="s">
         <v>67</v>
       </c>
       <c r="D24" s="1" t="s">
@@ -1846,7 +1865,7 @@
       </c>
       <c r="E24" s="1" t="str">
         <f t="shared" si="0"/>
-        <v>**Kamesh Madduri** Pennsylvania State University&lt;br&gt;</v>
+        <v>**Xin Liang** Oak Ridge National Laboratory&lt;br&gt;</v>
       </c>
     </row>
     <row r="25" ht="12" spans="1:5">
@@ -1864,17 +1883,17 @@
       </c>
       <c r="E25" s="1" t="str">
         <f t="shared" si="0"/>
-        <v>**Tanu Malik** DePaul University, Chicago&lt;br&gt;</v>
+        <v>**Kamesh Madduri** Pennsylvania State University&lt;br&gt;</v>
       </c>
     </row>
     <row r="26" ht="12" spans="1:5">
       <c r="A26" s="1" t="s">
         <v>71</v>
       </c>
-      <c r="B26" s="4" t="s">
+      <c r="B26" s="1" t="s">
         <v>72</v>
       </c>
-      <c r="C26" s="1" t="s">
+      <c r="C26" s="5" t="s">
         <v>73</v>
       </c>
       <c r="D26" s="1" t="s">
@@ -1882,7 +1901,7 @@
       </c>
       <c r="E26" s="1" t="str">
         <f t="shared" si="0"/>
-        <v>**Federica Mandreoli** Università degli Studi di Modena e Reggio Emilia, Italy&lt;br&gt;</v>
+        <v>**Tanu Malik** DePaul University, Chicago&lt;br&gt;</v>
       </c>
     </row>
     <row r="27" ht="12" spans="1:5">
@@ -1893,32 +1912,32 @@
         <v>75</v>
       </c>
       <c r="C27" s="1" t="s">
-        <v>64</v>
+        <v>76</v>
       </c>
       <c r="D27" s="1" t="s">
         <v>5</v>
       </c>
       <c r="E27" s="1" t="str">
         <f t="shared" si="0"/>
-        <v>**Kshitij Mehta** Oak Ridge National Laboratory&lt;br&gt;</v>
+        <v>**Federica Mandreoli** Università degli Studi di Modena e Reggio Emilia, Italy&lt;br&gt;</v>
       </c>
     </row>
     <row r="28" ht="12" spans="1:5">
       <c r="A28" s="1" t="s">
-        <v>76</v>
-      </c>
-      <c r="B28" s="1" t="s">
         <v>77</v>
       </c>
-      <c r="C28" s="5" t="s">
+      <c r="B28" s="4" t="s">
         <v>78</v>
       </c>
+      <c r="C28" s="1" t="s">
+        <v>67</v>
+      </c>
       <c r="D28" s="1" t="s">
         <v>5</v>
       </c>
       <c r="E28" s="1" t="str">
         <f t="shared" si="0"/>
-        <v>**Niccolo Meneghetti** University of Michigan - Dearborn&lt;br&gt;</v>
+        <v>**Kshitij Mehta** Oak Ridge National Laboratory&lt;br&gt;</v>
       </c>
     </row>
     <row r="29" ht="12" spans="1:5">
@@ -1936,7 +1955,7 @@
       </c>
       <c r="E29" s="1" t="str">
         <f t="shared" si="0"/>
-        <v>**Paolo Missier** Newcastle University&lt;br&gt;</v>
+        <v>**Niccolo Meneghetti** University of Michigan - Dearborn&lt;br&gt;</v>
       </c>
     </row>
     <row r="30" ht="12" spans="1:5">
@@ -1954,43 +1973,43 @@
       </c>
       <c r="E30" s="1" t="str">
         <f t="shared" si="0"/>
+        <v>**Paolo Missier** Newcastle University&lt;br&gt;</v>
+      </c>
+    </row>
+    <row r="31" ht="12" spans="1:5">
+      <c r="A31" s="1" t="s">
+        <v>85</v>
+      </c>
+      <c r="B31" s="1" t="s">
+        <v>86</v>
+      </c>
+      <c r="C31" s="5" t="s">
+        <v>87</v>
+      </c>
+      <c r="D31" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="E31" s="1" t="str">
+        <f t="shared" si="0"/>
         <v>**Bongki Moon** Seoul National University&lt;br&gt;</v>
       </c>
     </row>
-    <row r="31" ht="12" spans="1:5">
-      <c r="A31" s="6" t="s">
-        <v>85</v>
-      </c>
-      <c r="B31" s="6" t="s">
-        <v>86</v>
-      </c>
-      <c r="C31" s="6" t="s">
-        <v>87</v>
-      </c>
-      <c r="D31" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="E31" s="1" t="str">
+    <row r="32" ht="12" spans="1:5">
+      <c r="A32" s="7" t="s">
+        <v>88</v>
+      </c>
+      <c r="B32" s="7" t="s">
+        <v>89</v>
+      </c>
+      <c r="C32" s="7" t="s">
+        <v>90</v>
+      </c>
+      <c r="D32" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="E32" s="1" t="str">
         <f t="shared" si="0"/>
         <v>**Alexander Rasin** DePaul University&lt;br&gt;</v>
-      </c>
-    </row>
-    <row r="32" ht="12" spans="1:5">
-      <c r="A32" s="1" t="s">
-        <v>88</v>
-      </c>
-      <c r="B32" s="1" t="s">
-        <v>89</v>
-      </c>
-      <c r="C32" s="5" t="s">
-        <v>90</v>
-      </c>
-      <c r="D32" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="E32" s="1" t="str">
-        <f t="shared" si="0"/>
-        <v>**Tore Risch** Uppsala University. Sweden&lt;br&gt;</v>
       </c>
     </row>
     <row r="33" ht="12" spans="1:5">
@@ -2008,7 +2027,7 @@
       </c>
       <c r="E33" s="1" t="str">
         <f t="shared" si="0"/>
-        <v>**Florin Rusu** University of California, Merced&lt;br&gt;</v>
+        <v>**Tore Risch** Uppsala University. Sweden&lt;br&gt;</v>
       </c>
     </row>
     <row r="34" ht="12" spans="1:5">
@@ -2026,61 +2045,61 @@
       </c>
       <c r="E34" s="1" t="str">
         <f t="shared" si="0"/>
+        <v>**Florin Rusu** University of California, Merced&lt;br&gt;</v>
+      </c>
+    </row>
+    <row r="35" ht="12" spans="1:5">
+      <c r="A35" s="1" t="s">
+        <v>97</v>
+      </c>
+      <c r="B35" s="1" t="s">
+        <v>98</v>
+      </c>
+      <c r="C35" s="5" t="s">
+        <v>99</v>
+      </c>
+      <c r="D35" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="E35" s="1" t="str">
+        <f t="shared" si="0"/>
         <v>**Iulian Sandu-Popa** DAVID Laboratory, University of Versailles Saint-Quentin&lt;br&gt;</v>
       </c>
     </row>
-    <row r="35" ht="12" spans="1:5">
-      <c r="A35" s="6" t="s">
-        <v>97</v>
-      </c>
-      <c r="B35" s="6" t="s">
-        <v>98</v>
-      </c>
-      <c r="C35" s="6" t="s">
-        <v>99</v>
-      </c>
-      <c r="D35" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="E35" s="1" t="str">
+    <row r="36" ht="12" spans="1:5">
+      <c r="A36" s="7" t="s">
+        <v>100</v>
+      </c>
+      <c r="B36" s="7" t="s">
+        <v>101</v>
+      </c>
+      <c r="C36" s="7" t="s">
+        <v>102</v>
+      </c>
+      <c r="D36" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="E36" s="1" t="str">
         <f t="shared" si="0"/>
         <v>**Jagan Sankaranarayanan** Google Inc&lt;br&gt;</v>
       </c>
     </row>
-    <row r="36" ht="12" spans="1:5">
-      <c r="A36" s="6" t="s">
-        <v>100</v>
-      </c>
-      <c r="B36" s="6" t="s">
-        <v>101</v>
-      </c>
-      <c r="C36" s="6" t="s">
-        <v>102</v>
-      </c>
-      <c r="D36" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="E36" s="1" t="str">
+    <row r="37" ht="12" spans="1:5">
+      <c r="A37" s="7" t="s">
+        <v>103</v>
+      </c>
+      <c r="B37" s="7" t="s">
+        <v>104</v>
+      </c>
+      <c r="C37" s="7" t="s">
+        <v>105</v>
+      </c>
+      <c r="D37" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="E37" s="1" t="str">
         <f t="shared" si="0"/>
         <v>**Galen Shipman** Los Alamos National Laboratory&lt;br&gt;</v>
-      </c>
-    </row>
-    <row r="37" ht="12" spans="1:5">
-      <c r="A37" s="1" t="s">
-        <v>103</v>
-      </c>
-      <c r="B37" s="1" t="s">
-        <v>104</v>
-      </c>
-      <c r="C37" s="5" t="s">
-        <v>105</v>
-      </c>
-      <c r="D37" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="E37" s="1" t="str">
-        <f t="shared" si="0"/>
-        <v>**Tarique Siddiqui** Microsoft Research&lt;br&gt;</v>
       </c>
     </row>
     <row r="38" ht="12" spans="1:5">
@@ -2098,79 +2117,79 @@
       </c>
       <c r="E38" s="1" t="str">
         <f t="shared" si="0"/>
-        <v>**Kurt Stockinger** Zurich University of Applied Sciences&lt;br&gt;</v>
+        <v>**Tarique Siddiqui** Microsoft Research&lt;br&gt;</v>
       </c>
     </row>
     <row r="39" ht="12" spans="1:5">
-      <c r="A39" s="6" t="s">
+      <c r="A39" s="1" t="s">
         <v>109</v>
       </c>
       <c r="B39" s="1" t="s">
         <v>110</v>
       </c>
-      <c r="C39" s="6" t="s">
+      <c r="C39" s="5" t="s">
+        <v>111</v>
+      </c>
+      <c r="D39" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="E39" s="1" t="str">
+        <f>CONCATENATE("**",A39," ",B39,"** ",C39,D39)</f>
+        <v>**Kurt Stockinger** Zurich University of Applied Sciences&lt;br&gt;</v>
+      </c>
+    </row>
+    <row r="40" ht="12" spans="1:5">
+      <c r="A40" s="7" t="s">
+        <v>112</v>
+      </c>
+      <c r="B40" s="1" t="s">
+        <v>113</v>
+      </c>
+      <c r="C40" s="7" t="s">
         <v>14</v>
       </c>
-      <c r="D39" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="E39" s="1" t="str">
-        <f t="shared" si="0"/>
+      <c r="D40" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="E40" s="1" t="str">
+        <f>CONCATENATE("**",A40," ",B40,"** ",C40,D40)</f>
         <v>**Houjun Tang** Lawrence Berkeley National Laboratory&lt;br&gt;</v>
       </c>
     </row>
-    <row r="40" ht="12" spans="1:5">
-      <c r="A40" s="6" t="s">
-        <v>111</v>
-      </c>
-      <c r="B40" s="1" t="s">
-        <v>112</v>
-      </c>
-      <c r="C40" s="6" t="s">
-        <v>113</v>
-      </c>
-      <c r="D40" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="E40" s="1" t="str">
-        <f t="shared" si="0"/>
+    <row r="41" ht="12" spans="1:5">
+      <c r="A41" s="7" t="s">
+        <v>114</v>
+      </c>
+      <c r="B41" s="1" t="s">
+        <v>115</v>
+      </c>
+      <c r="C41" s="7" t="s">
+        <v>116</v>
+      </c>
+      <c r="D41" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="E41" s="1" t="str">
+        <f>CONCATENATE("**",A41," ",B41,"** ",C41,D41)</f>
         <v>**Douglas Thain** University of Notre Dame&lt;br&gt;</v>
-      </c>
-    </row>
-    <row r="41" ht="12" spans="1:5">
-      <c r="A41" s="1" t="s">
-        <v>114</v>
-      </c>
-      <c r="B41" s="4" t="s">
-        <v>115</v>
-      </c>
-      <c r="C41" s="1" t="s">
-        <v>116</v>
-      </c>
-      <c r="D41" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="E41" s="1" t="str">
-        <f t="shared" si="0"/>
-        <v>**Farouk Toumani** Limos-Blaise Pascal University, Clermont-Ferrand, France&lt;br&gt;</v>
       </c>
     </row>
     <row r="42" ht="12" spans="1:5">
       <c r="A42" s="1" t="s">
         <v>117</v>
       </c>
-      <c r="B42" s="1" t="s">
+      <c r="B42" s="4" t="s">
         <v>118</v>
       </c>
-      <c r="C42" s="5" t="s">
+      <c r="C42" s="1" t="s">
         <v>119</v>
       </c>
       <c r="D42" s="1" t="s">
         <v>5</v>
       </c>
       <c r="E42" s="1" t="str">
-        <f t="shared" si="0"/>
-        <v>**Yicheng Tu** University of South Florida&lt;br&gt;</v>
+        <f>CONCATENATE("**",A42," ",B42,"** ",C42,D42)</f>
+        <v>**Farouk Toumani** Limos-Blaise Pascal University, Clermont-Ferrand, France&lt;br&gt;</v>
       </c>
     </row>
     <row r="43" ht="12" spans="1:5">
@@ -2187,8 +2206,8 @@
         <v>5</v>
       </c>
       <c r="E43" s="1" t="str">
-        <f t="shared" si="0"/>
-        <v>**Marco Vieira** University of Coimbra, Portugal&lt;br&gt;</v>
+        <f>CONCATENATE("**",A43," ",B43,"** ",C43,D43)</f>
+        <v>**Yicheng Tu** University of South Florida&lt;br&gt;</v>
       </c>
     </row>
     <row r="44" ht="12" spans="1:5">
@@ -2199,50 +2218,50 @@
         <v>124</v>
       </c>
       <c r="C44" s="5" t="s">
-        <v>14</v>
+        <v>125</v>
       </c>
       <c r="D44" s="1" t="s">
         <v>5</v>
       </c>
       <c r="E44" s="1" t="str">
-        <f t="shared" si="0"/>
-        <v>**John Wu** Lawrence Berkeley National Laboratory&lt;br&gt;</v>
+        <f>CONCATENATE("**",A44," ",B44,"** ",C44,D44)</f>
+        <v>**Marco Vieira** University of Coimbra, Portugal&lt;br&gt;</v>
       </c>
     </row>
     <row r="45" ht="12" spans="1:5">
       <c r="A45" s="1" t="s">
-        <v>125</v>
-      </c>
-      <c r="B45" s="4" t="s">
-        <v>124</v>
-      </c>
-      <c r="C45" s="1" t="s">
         <v>126</v>
       </c>
+      <c r="B45" s="1" t="s">
+        <v>127</v>
+      </c>
+      <c r="C45" s="5" t="s">
+        <v>14</v>
+      </c>
       <c r="D45" s="1" t="s">
         <v>5</v>
       </c>
       <c r="E45" s="1" t="str">
-        <f t="shared" si="0"/>
-        <v>**Jia Wu** Macquarie University&lt;br&gt;</v>
+        <f>CONCATENATE("**",A45," ",B45,"** ",C45,D45)</f>
+        <v>**John Wu** Lawrence Berkeley National Laboratory&lt;br&gt;</v>
       </c>
     </row>
     <row r="46" ht="12" spans="1:5">
       <c r="A46" s="1" t="s">
+        <v>128</v>
+      </c>
+      <c r="B46" s="4" t="s">
         <v>127</v>
       </c>
-      <c r="B46" s="1" t="s">
-        <v>128</v>
-      </c>
-      <c r="C46" s="5" t="s">
+      <c r="C46" s="1" t="s">
         <v>129</v>
       </c>
       <c r="D46" s="1" t="s">
         <v>5</v>
       </c>
       <c r="E46" s="1" t="str">
-        <f t="shared" si="0"/>
-        <v>**Zichen Xu** The Nanchang University, Nanchang, China&lt;br&gt;</v>
+        <f>CONCATENATE("**",A46," ",B46,"** ",C46,D46)</f>
+        <v>**Jia Wu** Macquarie University&lt;br&gt;</v>
       </c>
     </row>
     <row r="47" ht="12" spans="1:5">
@@ -2259,8 +2278,8 @@
         <v>5</v>
       </c>
       <c r="E47" s="1" t="str">
-        <f t="shared" si="0"/>
-        <v>**Hongfeng Yu** University of Nebraska-Lincoln&lt;br&gt;</v>
+        <f>CONCATENATE("**",A47," ",B47,"** ",C47,D47)</f>
+        <v>**Zichen Xu** The Nanchang University, Nanchang, China&lt;br&gt;</v>
       </c>
     </row>
     <row r="48" ht="12" spans="1:5">
@@ -2277,8 +2296,8 @@
         <v>5</v>
       </c>
       <c r="E48" s="1" t="str">
-        <f t="shared" si="0"/>
-        <v>**Xuechen Zhang** Washington State Universit&lt;br&gt;</v>
+        <f>CONCATENATE("**",A48," ",B48,"** ",C48,D48)</f>
+        <v>**Hongfeng Yu** University of Nebraska-Lincoln&lt;br&gt;</v>
       </c>
     </row>
     <row r="49" ht="12" spans="1:5">
@@ -2289,37 +2308,55 @@
         <v>137</v>
       </c>
       <c r="C49" s="5" t="s">
-        <v>78</v>
+        <v>138</v>
       </c>
       <c r="D49" s="1" t="s">
         <v>5</v>
       </c>
       <c r="E49" s="1" t="str">
-        <f t="shared" si="0"/>
-        <v>**Qiang Zhu** University of Michigan - Dearborn&lt;br&gt;</v>
+        <f>CONCATENATE("**",A49," ",B49,"** ",C49,D49)</f>
+        <v>**Xuechen Zhang** Washington State Universit&lt;br&gt;</v>
       </c>
     </row>
     <row r="50" ht="12" spans="1:5">
       <c r="A50" s="1" t="s">
-        <v>125</v>
+        <v>139</v>
       </c>
       <c r="B50" s="1" t="s">
-        <v>138</v>
+        <v>140</v>
       </c>
       <c r="C50" s="5" t="s">
-        <v>139</v>
+        <v>81</v>
       </c>
       <c r="D50" s="1" t="s">
         <v>5</v>
       </c>
       <c r="E50" s="1" t="str">
-        <f t="shared" si="0"/>
+        <f>CONCATENATE("**",A50," ",B50,"** ",C50,D50)</f>
+        <v>**Qiang Zhu** University of Michigan - Dearborn&lt;br&gt;</v>
+      </c>
+    </row>
+    <row r="51" ht="12" spans="1:5">
+      <c r="A51" s="1" t="s">
+        <v>128</v>
+      </c>
+      <c r="B51" s="1" t="s">
+        <v>141</v>
+      </c>
+      <c r="C51" s="5" t="s">
+        <v>142</v>
+      </c>
+      <c r="D51" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="E51" s="1" t="str">
+        <f>CONCATENATE("**",A51," ",B51,"** ",C51,D51)</f>
         <v>**Jia Zou** Arizona State University&lt;br&gt;</v>
       </c>
     </row>
   </sheetData>
-  <sortState ref="A2:E50">
-    <sortCondition ref="B2:B50"/>
+  <sortState ref="A2:E52">
+    <sortCondition ref="B2:B52"/>
   </sortState>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.511805555555556" footer="0.511805555555556"/>
   <headerFooter/>

</xml_diff>